<commit_message>
add variable description in dictionary
</commit_message>
<xml_diff>
--- a/data-raw/dictionary.xlsx
+++ b/data-raw/dictionary.xlsx
@@ -1,169 +1,257 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svijay\Desktop\github\personal-phd\bcsa\data-raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E105A3-C4E0-47E6-BB4E-8749D440F548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
-  <si>
-    <t xml:space="preserve">directory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">file_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variable_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variable_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df_aae.rda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serial_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">session_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uv_bcc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blue_bcc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ir_bcc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uv_babs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blue_babs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ir_babs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">day_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exp_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emission_source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df_collocation.rda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">settlement_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time_of_day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type_of_settlement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df_mm.rda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id_road_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">collocation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dc_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dc_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type_of_road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df_mm_road_type.rda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df_pm.rda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df_pm_trips.rda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">df_sm.rda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">main_exp</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="75">
+  <si>
+    <t>directory</t>
+  </si>
+  <si>
+    <t>file_name</t>
+  </si>
+  <si>
+    <t>variable_name</t>
+  </si>
+  <si>
+    <t>variable_type</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>data/</t>
+  </si>
+  <si>
+    <t>df_aae.rda</t>
+  </si>
+  <si>
+    <t>serial_number</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>session_id</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>uv_bcc</t>
+  </si>
+  <si>
+    <t>blue_bcc</t>
+  </si>
+  <si>
+    <t>ir_bcc</t>
+  </si>
+  <si>
+    <t>uv_babs</t>
+  </si>
+  <si>
+    <t>blue_babs</t>
+  </si>
+  <si>
+    <t>ir_babs</t>
+  </si>
+  <si>
+    <t>date_time</t>
+  </si>
+  <si>
+    <t>day_type</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>date_start</t>
+  </si>
+  <si>
+    <t>date_end</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>end_time</t>
+  </si>
+  <si>
+    <t>exp_type</t>
+  </si>
+  <si>
+    <t>emission_source</t>
+  </si>
+  <si>
+    <t>df_collocation.rda</t>
+  </si>
+  <si>
+    <t>settlement_id</t>
+  </si>
+  <si>
+    <t>time_of_day</t>
+  </si>
+  <si>
+    <t>type_of_settlement</t>
+  </si>
+  <si>
+    <t>df_mm.rda</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>id_road_type</t>
+  </si>
+  <si>
+    <t>collocation</t>
+  </si>
+  <si>
+    <t>dc_1</t>
+  </si>
+  <si>
+    <t>dc_2</t>
+  </si>
+  <si>
+    <t>type_of_road</t>
+  </si>
+  <si>
+    <t>df_mm_road_type.rda</t>
+  </si>
+  <si>
+    <t>df_pm.rda</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>df_pm_trips.rda</t>
+  </si>
+  <si>
+    <t>df_sm.rda</t>
+  </si>
+  <si>
+    <t>main_exp</t>
+  </si>
+  <si>
+    <t>serial number of the MA200 monitoring from which the data is collected</t>
+  </si>
+  <si>
+    <t>session number of the MA200 monitor (each monitoring session is automatically given a number in the output file of MA200 monitoring data)</t>
+  </si>
+  <si>
+    <t>date of monitoring</t>
+  </si>
+  <si>
+    <t>time of monitoring</t>
+  </si>
+  <si>
+    <t>latitude of location of monitoring</t>
+  </si>
+  <si>
+    <t>longitude of location of monitoring</t>
+  </si>
+  <si>
+    <t>concentration of black carbon at the UV (ultravoilet) wavelength channel in ng/m3</t>
+  </si>
+  <si>
+    <t>concentration of black carbon at the Blue wavelength channel in ng/m3</t>
+  </si>
+  <si>
+    <t>concentration of black carbon at the IR (infrared) wavelength channel in ng/m3</t>
+  </si>
+  <si>
+    <t>absorption coefficient of black carbon at the UV (ultravoilet) wavelength channel</t>
+  </si>
+  <si>
+    <t>absorption coefficient of black carbon at the Blue wavelength channel</t>
+  </si>
+  <si>
+    <t>absorption coefficient of black carbon at the IR (infrared) wavelength channel</t>
+  </si>
+  <si>
+    <t>date and time of monitoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type of day of monitoring - weekend or weeday </t>
+  </si>
+  <si>
+    <t>id is a unique identifier given to every monitoring session and experiment given in the data structure</t>
+  </si>
+  <si>
+    <t>starting date of the experiment</t>
+  </si>
+  <si>
+    <t>end date of the experiment</t>
+  </si>
+  <si>
+    <t>starting time of the experiment</t>
+  </si>
+  <si>
+    <t>end time of the experiment</t>
+  </si>
+  <si>
+    <t>type of experiment</t>
+  </si>
+  <si>
+    <t>source of emission</t>
+  </si>
+  <si>
+    <t>the experiment phase during which the sensors were collocated</t>
+  </si>
+  <si>
+    <t>settlement name at which the monitoring was conducted</t>
+  </si>
+  <si>
+    <t>ending time of the experiment</t>
+  </si>
+  <si>
+    <t>type of settlement - formal or informal</t>
+  </si>
+  <si>
+    <t>the days are divided into three types - morning, first half and second half</t>
+  </si>
+  <si>
+    <t>ending date of the experiment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -172,12 +260,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -192,13 +286,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -480,14 +584,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E149"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -518,10 +624,10 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -535,10 +641,10 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -552,10 +658,10 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -569,10 +675,10 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -586,10 +692,10 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -603,10 +709,10 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -620,10 +726,10 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -637,10 +743,10 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -654,10 +760,10 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -671,10 +777,10 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -688,10 +794,10 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -705,10 +811,10 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -722,10 +828,10 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -739,10 +845,10 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -756,10 +862,10 @@
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -773,10 +879,10 @@
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -790,10 +896,10 @@
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -807,10 +913,10 @@
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -824,10 +930,10 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -841,10 +947,10 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -858,10 +964,10 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -875,10 +981,10 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -892,10 +998,10 @@
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -909,10 +1015,10 @@
         <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -926,10 +1032,10 @@
         <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -943,10 +1049,10 @@
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -960,10 +1066,10 @@
         <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -977,10 +1083,10 @@
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -994,10 +1100,10 @@
         <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1011,10 +1117,10 @@
         <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1028,10 +1134,10 @@
         <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1045,10 +1151,10 @@
         <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1062,10 +1168,10 @@
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1079,10 +1185,10 @@
         <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1096,10 +1202,10 @@
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1113,10 +1219,10 @@
         <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1130,10 +1236,10 @@
         <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1147,10 +1253,10 @@
         <v>11</v>
       </c>
       <c r="E39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1164,10 +1270,10 @@
         <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1181,10 +1287,10 @@
         <v>11</v>
       </c>
       <c r="E41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -1198,10 +1304,10 @@
         <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1209,50 +1315,50 @@
         <v>31</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E45" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -1260,16 +1366,16 @@
         <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1277,16 +1383,16 @@
         <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
       </c>
       <c r="E47" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -1294,16 +1400,16 @@
         <v>35</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
       </c>
       <c r="E48" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1311,16 +1417,16 @@
         <v>35</v>
       </c>
       <c r="C49" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1328,16 +1434,16 @@
         <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
       </c>
       <c r="E50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1345,16 +1451,16 @@
         <v>35</v>
       </c>
       <c r="C51" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
       <c r="E51" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1362,16 +1468,16 @@
         <v>35</v>
       </c>
       <c r="C52" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
       </c>
       <c r="E52" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -1379,16 +1485,16 @@
         <v>35</v>
       </c>
       <c r="C53" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
       </c>
       <c r="E53" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -1396,16 +1502,16 @@
         <v>35</v>
       </c>
       <c r="C54" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
       </c>
       <c r="E54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -1413,16 +1519,16 @@
         <v>35</v>
       </c>
       <c r="C55" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -1430,16 +1536,16 @@
         <v>35</v>
       </c>
       <c r="C56" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
       </c>
       <c r="E56" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -1447,16 +1553,16 @@
         <v>35</v>
       </c>
       <c r="C57" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D57" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -1464,16 +1570,16 @@
         <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -1481,16 +1587,16 @@
         <v>35</v>
       </c>
       <c r="C59" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D59" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E59" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1498,16 +1604,16 @@
         <v>35</v>
       </c>
       <c r="C60" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
       </c>
       <c r="E60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -1515,67 +1621,64 @@
         <v>35</v>
       </c>
       <c r="C61" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D61" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E61" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C62" t="s">
-        <v>26</v>
-      </c>
-      <c r="D62" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="C62" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C63" t="s">
-        <v>29</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="C63" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E63" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C64" t="s">
-        <v>30</v>
-      </c>
-      <c r="D64" t="s">
-        <v>8</v>
+      <c r="C64" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E64" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -1583,16 +1686,16 @@
         <v>35</v>
       </c>
       <c r="C65" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D65" t="s">
         <v>8</v>
       </c>
       <c r="E65" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -1600,67 +1703,67 @@
         <v>35</v>
       </c>
       <c r="C66" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D66" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E66" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
-        <v>5</v>
-      </c>
-      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C67" t="s">
-        <v>32</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="C67" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E67" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="s">
-        <v>5</v>
-      </c>
-      <c r="B68" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C68" t="s">
-        <v>33</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="C68" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E68" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" t="s">
-        <v>5</v>
-      </c>
-      <c r="B69" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C69" t="s">
-        <v>38</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="C69" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E69" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -1668,16 +1771,16 @@
         <v>35</v>
       </c>
       <c r="C70" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D70" t="s">
         <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -1685,16 +1788,16 @@
         <v>35</v>
       </c>
       <c r="C71" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D71" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E71" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -1702,67 +1805,67 @@
         <v>35</v>
       </c>
       <c r="C72" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D72" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E72" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>5</v>
-      </c>
-      <c r="B73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C73" t="s">
-        <v>27</v>
-      </c>
-      <c r="D73" t="s">
-        <v>11</v>
+      <c r="C73" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E73" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>5</v>
       </c>
       <c r="B74" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C74" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D74" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E74" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>5</v>
       </c>
       <c r="B75" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C75" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E75" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -1770,16 +1873,16 @@
         <v>42</v>
       </c>
       <c r="C76" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D76" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E76" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -1787,16 +1890,16 @@
         <v>42</v>
       </c>
       <c r="C77" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D77" t="s">
         <v>11</v>
       </c>
       <c r="E77" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -1804,16 +1907,16 @@
         <v>42</v>
       </c>
       <c r="C78" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D78" t="s">
         <v>11</v>
       </c>
       <c r="E78" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -1821,16 +1924,16 @@
         <v>42</v>
       </c>
       <c r="C79" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D79" t="s">
         <v>11</v>
       </c>
       <c r="E79" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="80">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -1838,16 +1941,16 @@
         <v>42</v>
       </c>
       <c r="C80" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D80" t="s">
         <v>11</v>
       </c>
       <c r="E80" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -1855,16 +1958,16 @@
         <v>42</v>
       </c>
       <c r="C81" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D81" t="s">
         <v>11</v>
       </c>
       <c r="E81" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>5</v>
       </c>
@@ -1872,16 +1975,16 @@
         <v>42</v>
       </c>
       <c r="C82" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D82" t="s">
         <v>11</v>
       </c>
       <c r="E82" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="83">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -1889,16 +1992,16 @@
         <v>42</v>
       </c>
       <c r="C83" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D83" t="s">
         <v>11</v>
       </c>
       <c r="E83" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="84">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>5</v>
       </c>
@@ -1906,16 +2009,16 @@
         <v>42</v>
       </c>
       <c r="C84" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D84" t="s">
         <v>11</v>
       </c>
       <c r="E84" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="85">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -1923,16 +2026,16 @@
         <v>42</v>
       </c>
       <c r="C85" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D85" t="s">
         <v>11</v>
       </c>
       <c r="E85" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -1940,16 +2043,16 @@
         <v>42</v>
       </c>
       <c r="C86" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D86" t="s">
         <v>11</v>
       </c>
       <c r="E86" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -1957,16 +2060,16 @@
         <v>42</v>
       </c>
       <c r="C87" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D87" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E87" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -1974,16 +2077,16 @@
         <v>42</v>
       </c>
       <c r="C88" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D88" t="s">
         <v>11</v>
       </c>
       <c r="E88" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="89">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -1991,16 +2094,16 @@
         <v>42</v>
       </c>
       <c r="C89" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D89" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E89" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -2008,16 +2111,16 @@
         <v>42</v>
       </c>
       <c r="C90" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D90" t="s">
         <v>11</v>
       </c>
       <c r="E90" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="91">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -2025,16 +2128,16 @@
         <v>42</v>
       </c>
       <c r="C91" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D91" t="s">
         <v>11</v>
       </c>
       <c r="E91" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="92">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>5</v>
       </c>
@@ -2042,16 +2145,16 @@
         <v>42</v>
       </c>
       <c r="C92" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D92" t="s">
         <v>11</v>
       </c>
       <c r="E92" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="93">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>5</v>
       </c>
@@ -2059,16 +2162,16 @@
         <v>42</v>
       </c>
       <c r="C93" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D93" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E93" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="94">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -2076,16 +2179,16 @@
         <v>42</v>
       </c>
       <c r="C94" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D94" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E94" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>5</v>
       </c>
@@ -2093,16 +2196,16 @@
         <v>42</v>
       </c>
       <c r="C95" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D95" t="s">
         <v>8</v>
       </c>
       <c r="E95" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="96">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>5</v>
       </c>
@@ -2110,50 +2213,50 @@
         <v>42</v>
       </c>
       <c r="C96" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D96" t="s">
         <v>8</v>
       </c>
       <c r="E96" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>5</v>
       </c>
       <c r="B97" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C97" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D97" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E97" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="98">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C98" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D98" t="s">
         <v>8</v>
       </c>
       <c r="E98" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="99">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>5</v>
       </c>
@@ -2161,16 +2264,16 @@
         <v>43</v>
       </c>
       <c r="C99" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D99" t="s">
         <v>11</v>
       </c>
       <c r="E99" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="100">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>5</v>
       </c>
@@ -2178,16 +2281,16 @@
         <v>43</v>
       </c>
       <c r="C100" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D100" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E100" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="101">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>5</v>
       </c>
@@ -2195,16 +2298,16 @@
         <v>43</v>
       </c>
       <c r="C101" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D101" t="s">
         <v>11</v>
       </c>
       <c r="E101" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="102">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>5</v>
       </c>
@@ -2212,16 +2315,16 @@
         <v>43</v>
       </c>
       <c r="C102" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D102" t="s">
         <v>11</v>
       </c>
       <c r="E102" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="103">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>5</v>
       </c>
@@ -2229,16 +2332,16 @@
         <v>43</v>
       </c>
       <c r="C103" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D103" t="s">
         <v>11</v>
       </c>
       <c r="E103" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="104">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>5</v>
       </c>
@@ -2246,50 +2349,46 @@
         <v>43</v>
       </c>
       <c r="C104" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D104" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E104" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s">
-        <v>5</v>
-      </c>
-      <c r="B105" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C105" t="s">
-        <v>28</v>
-      </c>
-      <c r="D105" t="s">
-        <v>11</v>
-      </c>
-      <c r="E105" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s">
-        <v>5</v>
-      </c>
-      <c r="B106" t="s">
+      <c r="C105" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="1"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C106" t="s">
-        <v>29</v>
-      </c>
-      <c r="D106" t="s">
-        <v>8</v>
-      </c>
-      <c r="E106" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="107">
+      <c r="C106" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E106" s="1"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>5</v>
       </c>
@@ -2297,50 +2396,50 @@
         <v>43</v>
       </c>
       <c r="C107" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D107" t="s">
         <v>8</v>
       </c>
       <c r="E107" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="108">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>5</v>
       </c>
       <c r="B108" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C108" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D108" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E108" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="109">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>5</v>
       </c>
       <c r="B109" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C109" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D109" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E109" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="110">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>5</v>
       </c>
@@ -2348,16 +2447,16 @@
         <v>45</v>
       </c>
       <c r="C110" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D110" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E110" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="111">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>5</v>
       </c>
@@ -2365,16 +2464,16 @@
         <v>45</v>
       </c>
       <c r="C111" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D111" t="s">
         <v>11</v>
       </c>
       <c r="E111" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="112">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>5</v>
       </c>
@@ -2382,16 +2481,16 @@
         <v>45</v>
       </c>
       <c r="C112" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D112" t="s">
         <v>11</v>
       </c>
       <c r="E112" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="113">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>5</v>
       </c>
@@ -2399,16 +2498,16 @@
         <v>45</v>
       </c>
       <c r="C113" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D113" t="s">
         <v>11</v>
       </c>
       <c r="E113" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="114">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>5</v>
       </c>
@@ -2416,16 +2515,16 @@
         <v>45</v>
       </c>
       <c r="C114" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D114" t="s">
         <v>11</v>
       </c>
       <c r="E114" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="115">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>5</v>
       </c>
@@ -2433,16 +2532,16 @@
         <v>45</v>
       </c>
       <c r="C115" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D115" t="s">
         <v>11</v>
       </c>
       <c r="E115" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="116">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>5</v>
       </c>
@@ -2450,16 +2549,16 @@
         <v>45</v>
       </c>
       <c r="C116" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D116" t="s">
         <v>11</v>
       </c>
       <c r="E116" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="117">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>5</v>
       </c>
@@ -2467,16 +2566,16 @@
         <v>45</v>
       </c>
       <c r="C117" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D117" t="s">
         <v>11</v>
       </c>
       <c r="E117" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="118">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>5</v>
       </c>
@@ -2484,16 +2583,16 @@
         <v>45</v>
       </c>
       <c r="C118" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D118" t="s">
         <v>11</v>
       </c>
       <c r="E118" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="119">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>5</v>
       </c>
@@ -2501,16 +2600,16 @@
         <v>45</v>
       </c>
       <c r="C119" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D119" t="s">
         <v>11</v>
       </c>
       <c r="E119" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="120">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>5</v>
       </c>
@@ -2518,16 +2617,16 @@
         <v>45</v>
       </c>
       <c r="C120" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D120" t="s">
         <v>11</v>
       </c>
       <c r="E120" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="121">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>5</v>
       </c>
@@ -2535,16 +2634,16 @@
         <v>45</v>
       </c>
       <c r="C121" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D121" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E121" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="122">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>5</v>
       </c>
@@ -2552,16 +2651,16 @@
         <v>45</v>
       </c>
       <c r="C122" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D122" t="s">
         <v>11</v>
       </c>
       <c r="E122" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="123">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>5</v>
       </c>
@@ -2569,16 +2668,16 @@
         <v>45</v>
       </c>
       <c r="C123" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D123" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E123" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="124">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>5</v>
       </c>
@@ -2586,16 +2685,16 @@
         <v>45</v>
       </c>
       <c r="C124" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D124" t="s">
         <v>11</v>
       </c>
       <c r="E124" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="125">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>5</v>
       </c>
@@ -2603,16 +2702,16 @@
         <v>45</v>
       </c>
       <c r="C125" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D125" t="s">
         <v>11</v>
       </c>
       <c r="E125" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="126">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>5</v>
       </c>
@@ -2620,16 +2719,16 @@
         <v>45</v>
       </c>
       <c r="C126" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D126" t="s">
         <v>11</v>
       </c>
       <c r="E126" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="127">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>5</v>
       </c>
@@ -2637,16 +2736,16 @@
         <v>45</v>
       </c>
       <c r="C127" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D127" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E127" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="128">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>5</v>
       </c>
@@ -2654,50 +2753,50 @@
         <v>45</v>
       </c>
       <c r="C128" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D128" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E128" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="129">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>5</v>
       </c>
       <c r="B129" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C129" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D129" t="s">
         <v>8</v>
       </c>
       <c r="E129" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="130">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>5</v>
       </c>
       <c r="B130" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C130" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D130" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E130" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="131">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>5</v>
       </c>
@@ -2705,16 +2804,16 @@
         <v>46</v>
       </c>
       <c r="C131" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D131" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E131" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="132">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>5</v>
       </c>
@@ -2722,16 +2821,16 @@
         <v>46</v>
       </c>
       <c r="C132" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D132" t="s">
         <v>11</v>
       </c>
       <c r="E132" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="133">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>5</v>
       </c>
@@ -2739,16 +2838,16 @@
         <v>46</v>
       </c>
       <c r="C133" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D133" t="s">
         <v>11</v>
       </c>
       <c r="E133" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="134">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>5</v>
       </c>
@@ -2756,16 +2855,16 @@
         <v>46</v>
       </c>
       <c r="C134" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D134" t="s">
         <v>11</v>
       </c>
       <c r="E134" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="135">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>5</v>
       </c>
@@ -2773,16 +2872,16 @@
         <v>46</v>
       </c>
       <c r="C135" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D135" t="s">
         <v>11</v>
       </c>
       <c r="E135" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="136">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>5</v>
       </c>
@@ -2790,16 +2889,16 @@
         <v>46</v>
       </c>
       <c r="C136" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D136" t="s">
         <v>11</v>
       </c>
       <c r="E136" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="137">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>5</v>
       </c>
@@ -2807,16 +2906,16 @@
         <v>46</v>
       </c>
       <c r="C137" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D137" t="s">
         <v>11</v>
       </c>
       <c r="E137" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="138">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>5</v>
       </c>
@@ -2824,16 +2923,16 @@
         <v>46</v>
       </c>
       <c r="C138" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D138" t="s">
         <v>11</v>
       </c>
       <c r="E138" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="139">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>5</v>
       </c>
@@ -2841,16 +2940,16 @@
         <v>46</v>
       </c>
       <c r="C139" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D139" t="s">
         <v>11</v>
       </c>
       <c r="E139" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="140">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>5</v>
       </c>
@@ -2858,16 +2957,16 @@
         <v>46</v>
       </c>
       <c r="C140" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D140" t="s">
         <v>11</v>
       </c>
       <c r="E140" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="141">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>5</v>
       </c>
@@ -2875,16 +2974,16 @@
         <v>46</v>
       </c>
       <c r="C141" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D141" t="s">
         <v>11</v>
       </c>
       <c r="E141" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="142">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>5</v>
       </c>
@@ -2892,16 +2991,16 @@
         <v>46</v>
       </c>
       <c r="C142" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D142" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E142" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="143">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>5</v>
       </c>
@@ -2909,16 +3008,16 @@
         <v>46</v>
       </c>
       <c r="C143" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D143" t="s">
         <v>11</v>
       </c>
       <c r="E143" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="144">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>5</v>
       </c>
@@ -2926,16 +3025,16 @@
         <v>46</v>
       </c>
       <c r="C144" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D144" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E144" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="145">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>5</v>
       </c>
@@ -2943,16 +3042,16 @@
         <v>46</v>
       </c>
       <c r="C145" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D145" t="s">
         <v>11</v>
       </c>
       <c r="E145" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="146">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>5</v>
       </c>
@@ -2960,16 +3059,16 @@
         <v>46</v>
       </c>
       <c r="C146" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D146" t="s">
         <v>11</v>
       </c>
       <c r="E146" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="147">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>5</v>
       </c>
@@ -2977,16 +3076,16 @@
         <v>46</v>
       </c>
       <c r="C147" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D147" t="s">
         <v>11</v>
       </c>
       <c r="E147" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="148">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>5</v>
       </c>
@@ -2994,16 +3093,16 @@
         <v>46</v>
       </c>
       <c r="C148" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D148" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E148" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="149">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>5</v>
       </c>
@@ -3011,51 +3110,17 @@
         <v>46</v>
       </c>
       <c r="C149" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D149" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E149" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="s">
-        <v>5</v>
-      </c>
-      <c r="B150" t="s">
-        <v>46</v>
-      </c>
-      <c r="C150" t="s">
-        <v>29</v>
-      </c>
-      <c r="D150" t="s">
-        <v>8</v>
-      </c>
-      <c r="E150" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="s">
-        <v>5</v>
-      </c>
-      <c r="B151" t="s">
-        <v>46</v>
-      </c>
-      <c r="C151" t="s">
-        <v>47</v>
-      </c>
-      <c r="D151" t="s">
-        <v>8</v>
-      </c>
-      <c r="E151" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>